<commit_message>
Hema: EmployeeMangement,Test Util,Test Data Files
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/Automation Input File.xlsx
+++ b/src/main/java/testdata/Automation Input File.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="19875" windowHeight="7470" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="315" windowWidth="19875" windowHeight="7470" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="DetailsPage" sheetId="17" r:id="rId1"/>
@@ -17,17 +17,19 @@
     <sheet name="T1AddEmployee" sheetId="9" r:id="rId8"/>
     <sheet name="ExistingEmployee" sheetId="18" r:id="rId9"/>
     <sheet name="T1EditAddEmployee" sheetId="11" r:id="rId10"/>
-    <sheet name="T1ImportEmployee" sheetId="10" r:id="rId11"/>
-    <sheet name="T1WorkClasses" sheetId="14" r:id="rId12"/>
-    <sheet name="T1ManualPayroll" sheetId="15" r:id="rId13"/>
-    <sheet name="T1EditPayroll" sheetId="16" r:id="rId14"/>
+    <sheet name="T1EditImportEmployee" sheetId="19" r:id="rId11"/>
+    <sheet name="T1ImportEmployee" sheetId="10" r:id="rId12"/>
+    <sheet name="T1WorkClasses" sheetId="14" r:id="rId13"/>
+    <sheet name="T1ManualPayroll" sheetId="15" r:id="rId14"/>
+    <sheet name="T1EditPayroll" sheetId="16" r:id="rId15"/>
+    <sheet name="Sheet1" sheetId="20" r:id="rId16"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="307">
   <si>
     <t>EIN</t>
   </si>
@@ -866,31 +868,88 @@
     <t>06/20/2022</t>
   </si>
   <si>
-    <t>1425481452</t>
-  </si>
-  <si>
-    <t>Aliya</t>
-  </si>
-  <si>
-    <t>Manasa</t>
-  </si>
-  <si>
-    <t>1248</t>
-  </si>
-  <si>
-    <t>124578</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
-    <t>Manasa, Aliya, s</t>
-  </si>
-  <si>
-    <t>Aliyaa</t>
-  </si>
-  <si>
-    <t>Manasa, Aliyaa, s</t>
+    <t>06/28/2022</t>
+  </si>
+  <si>
+    <t>Apprentice Number</t>
+  </si>
+  <si>
+    <t>07/31/2023</t>
+  </si>
+  <si>
+    <t>FullName1</t>
+  </si>
+  <si>
+    <t>FullName2</t>
+  </si>
+  <si>
+    <t>04/01/2022</t>
+  </si>
+  <si>
+    <t>08/20/2022</t>
+  </si>
+  <si>
+    <t>10/20/2022</t>
+  </si>
+  <si>
+    <t>135417</t>
+  </si>
+  <si>
+    <t>Part Time Worker</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Johnee</t>
+  </si>
+  <si>
+    <t>6172</t>
+  </si>
+  <si>
+    <t>41145526</t>
+  </si>
+  <si>
+    <t>Bottle Washer-name - Apprentice</t>
+  </si>
+  <si>
+    <t>Bicycle Mechanic - Apprentice</t>
+  </si>
+  <si>
+    <t>Anitha</t>
+  </si>
+  <si>
+    <t>Parthu</t>
+  </si>
+  <si>
+    <t>5124</t>
+  </si>
+  <si>
+    <t>151417425</t>
+  </si>
+  <si>
+    <t>Parthu, Anitha, s</t>
+  </si>
+  <si>
+    <t>Anithaa</t>
+  </si>
+  <si>
+    <t>Parthu, Anithaa, s</t>
+  </si>
+  <si>
+    <t>Suresh, John, w</t>
+  </si>
+  <si>
+    <t>Gani, Rajesh, T</t>
+  </si>
+  <si>
+    <t>Cell Phone Repair - Apprentice</t>
+  </si>
+  <si>
+    <t>Rani, Anirudh, r</t>
   </si>
 </sst>
 </file>
@@ -900,7 +959,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -969,6 +1028,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0288D1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -991,7 +1056,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1011,6 +1076,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1391,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1466,10 +1532,10 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="18" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>275</v>
@@ -1523,7 +1589,7 @@
         <v>101</v>
       </c>
       <c r="T2" s="18" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -1533,6 +1599,205 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC2"/>
+  <sheetViews>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="A1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="K2" t="s">
+        <v>305</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q2">
+        <v>10</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="T2" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="V2" t="s">
+        <v>295</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -1654,7 +1919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1716,7 +1981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -1909,7 +2174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
@@ -2035,6 +2300,175 @@
       </c>
       <c r="S2" s="6" t="s">
         <v>210</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AZ1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:52" ht="17.25">
+      <c r="A1" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="L1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="R1" s="2"/>
+      <c r="S1" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AH1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="AI1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="AJ1" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="AK1" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="AP1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="AR1" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AT1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="AW1" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AX1" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="AY1" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2680,8 +3114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2853,19 +3287,19 @@
     </row>
     <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="6" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="B2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="F2" t="s">
         <v>27</v>
@@ -2957,7 +3391,7 @@
         <v>264</v>
       </c>
       <c r="AK2" s="10" t="s">
-        <v>139</v>
+        <v>294</v>
       </c>
       <c r="AL2" s="4" t="s">
         <v>119</v>
@@ -2978,7 +3412,7 @@
         <v>157</v>
       </c>
       <c r="AR2" s="10" t="s">
-        <v>152</v>
+        <v>295</v>
       </c>
       <c r="AS2" s="4" t="s">
         <v>158</v>
@@ -3073,22 +3507,22 @@
     </row>
     <row r="2" spans="1:16" ht="17.25">
       <c r="A2" s="18" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="C2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D2" t="s">
-        <v>281</v>
+        <v>279</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="G2" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Hema: Employee Management,Automation Input file
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/Automation Input File.xlsx
+++ b/src/main/java/testdata/Automation Input File.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="19875" windowHeight="7470" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="315" windowWidth="19875" windowHeight="7470" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="DetailsPage" sheetId="17" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="312">
   <si>
     <t>EIN</t>
   </si>
@@ -724,21 +724,9 @@
     <t>DT2</t>
   </si>
   <si>
-    <t>3/7/2022 (Mon)</t>
-  </si>
-  <si>
-    <t>3/10/2022 (Thu)</t>
-  </si>
-  <si>
-    <t>3/12/2022 (Sat)</t>
-  </si>
-  <si>
     <t>Day4</t>
   </si>
   <si>
-    <t>3/11/2022 (Fri)</t>
-  </si>
-  <si>
     <t>OT4</t>
   </si>
   <si>
@@ -931,25 +919,52 @@
     <t>151417425</t>
   </si>
   <si>
-    <t>Parthu, Anitha, s</t>
-  </si>
-  <si>
-    <t>Anithaa</t>
-  </si>
-  <si>
-    <t>Parthu, Anithaa, s</t>
-  </si>
-  <si>
-    <t>Suresh, John, w</t>
-  </si>
-  <si>
-    <t>Gani, Rajesh, T</t>
-  </si>
-  <si>
     <t>Cell Phone Repair - Apprentice</t>
   </si>
   <si>
-    <t>Rani, Anirudh, r</t>
+    <t>Anandh</t>
+  </si>
+  <si>
+    <t>Anandh, Mohan, s</t>
+  </si>
+  <si>
+    <t>Mohana</t>
+  </si>
+  <si>
+    <t>5852</t>
+  </si>
+  <si>
+    <t>512477253</t>
+  </si>
+  <si>
+    <t>Anandh, Mohana, s</t>
+  </si>
+  <si>
+    <t>Mohan</t>
+  </si>
+  <si>
+    <t>Suren, Johnny, w</t>
+  </si>
+  <si>
+    <t>Ranish, Anil, r</t>
+  </si>
+  <si>
+    <t>Gani, Raina, T</t>
+  </si>
+  <si>
+    <t>7/25/2022 (Mon)</t>
+  </si>
+  <si>
+    <t>7/28/2022 (Thu)</t>
+  </si>
+  <si>
+    <t>7/31/2022 (Sun)</t>
+  </si>
+  <si>
+    <t>7/27/2022 (Wed)</t>
+  </si>
+  <si>
+    <t>07/25/2022 - 07/31/2022</t>
   </si>
 </sst>
 </file>
@@ -959,7 +974,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1028,12 +1043,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0288D1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1056,7 +1065,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1076,7 +1085,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1393,10 +1401,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C1" t="s">
         <v>111</v>
@@ -1408,13 +1416,13 @@
         <v>66</v>
       </c>
       <c r="F1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="G1" t="s">
         <v>114</v>
       </c>
       <c r="H1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I1" t="s">
         <v>145</v>
@@ -1422,26 +1430,26 @@
     </row>
     <row r="2" spans="1:9" ht="16.5">
       <c r="A2" s="16" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="16" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>101</v>
@@ -1455,20 +1463,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>189</v>
       </c>
@@ -1482,114 +1490,108 @@
         <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>121</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="T1" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:19">
       <c r="A2" s="18" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>119</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F2" t="s">
         <v>190</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>191</v>
+      <c r="G2" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="J2" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>139</v>
+      <c r="K2" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="N2" s="6">
+        <v>20</v>
+      </c>
       <c r="O2" s="6">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="P2" s="6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="6">
         <v>10</v>
       </c>
-      <c r="R2" s="6">
-        <v>10</v>
-      </c>
-      <c r="S2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="T2" s="18" t="s">
-        <v>302</v>
+      <c r="S2" s="18" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -1602,8 +1604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1618,16 +1620,16 @@
         <v>189</v>
       </c>
       <c r="B1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D1" t="s">
         <v>125</v>
       </c>
       <c r="E1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>126</v>
@@ -1669,7 +1671,7 @@
         <v>144</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>134</v>
@@ -1699,24 +1701,24 @@
         <v>143</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:29">
-      <c r="A2" s="19" t="s">
-        <v>303</v>
+      <c r="A2" s="10" t="s">
+        <v>305</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>122</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>191</v>
@@ -1725,22 +1727,22 @@
         <v>100</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="10" t="s">
         <v>138</v>
       </c>
       <c r="K2" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>157</v>
@@ -1755,25 +1757,25 @@
         <v>10</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="S2" s="10" t="s">
         <v>304</v>
       </c>
       <c r="T2" s="15" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="U2" s="15" t="s">
         <v>193</v>
       </c>
       <c r="V2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="Y2" s="6" t="s">
         <v>63</v>
@@ -1787,7 +1789,7 @@
       <c r="AB2" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AC2" s="10" t="s">
         <v>306</v>
       </c>
     </row>
@@ -1985,8 +1987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1:AN3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2061,33 +2063,33 @@
         <v>225</v>
       </c>
       <c r="V1" t="s">
+        <v>231</v>
+      </c>
+      <c r="W1" t="s">
         <v>234</v>
       </c>
-      <c r="W1" t="s">
-        <v>238</v>
-      </c>
       <c r="X1" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>233</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB1" t="s">
         <v>236</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>239</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>241</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:28">
-      <c r="A2" s="6" t="s">
-        <v>213</v>
+      <c r="A2" s="12" t="s">
+        <v>311</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>231</v>
+        <v>307</v>
       </c>
       <c r="C2">
         <v>10.5</v>
@@ -2102,7 +2104,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>232</v>
+        <v>308</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2113,8 +2115,8 @@
       <c r="J2">
         <v>5</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>233</v>
+      <c r="K2" s="12" t="s">
+        <v>309</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>157</v>
@@ -2146,8 +2148,8 @@
       <c r="U2">
         <v>200</v>
       </c>
-      <c r="V2" s="6" t="s">
-        <v>235</v>
+      <c r="V2" s="12" t="s">
+        <v>310</v>
       </c>
       <c r="W2">
         <v>10</v>
@@ -2192,7 +2194,7 @@
         <v>189</v>
       </c>
       <c r="C1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D1" t="s">
         <v>217</v>
@@ -2231,7 +2233,7 @@
         <v>225</v>
       </c>
       <c r="P1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="Q1" t="s">
         <v>217</v>
@@ -2240,7 +2242,7 @@
         <v>215</v>
       </c>
       <c r="S1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -2248,10 +2250,10 @@
         <v>213</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D2">
         <v>10.5</v>
@@ -2290,7 +2292,7 @@
         <v>200</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>157</v>
@@ -2319,19 +2321,19 @@
   <sheetData>
     <row r="1" spans="1:52" ht="17.25">
       <c r="A1" s="6" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F1" t="s">
         <v>27</v>
@@ -2365,11 +2367,11 @@
         <v>158</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="R1" s="2"/>
       <c r="S1" s="16" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="T1" s="17" t="s">
         <v>51</v>
@@ -2378,16 +2380,16 @@
         <v>53</v>
       </c>
       <c r="V1" s="16" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>56</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Z1" t="s">
         <v>122</v>
@@ -2420,7 +2422,7 @@
         <v>138</v>
       </c>
       <c r="AJ1" s="15" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AK1" s="10" t="s">
         <v>139</v>
@@ -2465,10 +2467,10 @@
         <v>161</v>
       </c>
       <c r="AY1" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="AZ1" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2644,13 +2646,13 @@
     </row>
     <row r="2" spans="1:50">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -2736,7 +2738,7 @@
         <v>82</v>
       </c>
       <c r="AG2" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="AH2" s="7" t="s">
         <v>93</v>
@@ -2766,13 +2768,13 @@
         <v>205</v>
       </c>
       <c r="AQ2" s="8" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="AR2" t="s">
         <v>10</v>
       </c>
       <c r="AS2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="AT2" t="s">
         <v>13</v>
@@ -2781,7 +2783,7 @@
         <v>15</v>
       </c>
       <c r="AV2" s="8" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="AW2" t="s">
         <v>16</v>
@@ -3114,8 +3116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3189,7 +3191,7 @@
         <v>112</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>113</v>
@@ -3198,10 +3200,10 @@
         <v>114</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>121</v>
@@ -3234,7 +3236,7 @@
         <v>125</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>96</v>
@@ -3287,19 +3289,19 @@
     </row>
     <row r="2" spans="1:52" ht="17.25">
       <c r="A2" s="6" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>297</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="F2" t="s">
         <v>27</v>
@@ -3333,11 +3335,11 @@
         <v>158</v>
       </c>
       <c r="Q2" s="16" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="16" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="T2" s="17" t="s">
         <v>51</v>
@@ -3346,16 +3348,16 @@
         <v>53</v>
       </c>
       <c r="V2" s="16" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="W2" s="4" t="s">
         <v>56</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Z2" t="s">
         <v>122</v>
@@ -3388,10 +3390,10 @@
         <v>138</v>
       </c>
       <c r="AJ2" s="15" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AK2" s="10" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="AL2" s="4" t="s">
         <v>119</v>
@@ -3412,7 +3414,7 @@
         <v>157</v>
       </c>
       <c r="AR2" s="10" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="AS2" s="4" t="s">
         <v>158</v>
@@ -3433,10 +3435,10 @@
         <v>161</v>
       </c>
       <c r="AY2" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="AZ2" s="4" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -3507,22 +3509,22 @@
     </row>
     <row r="2" spans="1:16" ht="17.25">
       <c r="A2" s="18" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="G2" t="s">
         <v>27</v>

</xml_diff>